<commit_message>
feat-prepare: (Competition and Referee templates), (Excel parser)
</commit_message>
<xml_diff>
--- a/Resources/Template_Referee.xlsx
+++ b/Resources/Template_Referee.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igor\Programming\Femida\Femida_v0.3\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B8A4E-81DB-4465-AFB4-B34FEA40DCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E3FB89-E197-42F3-8D9D-5D841D36FBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заполнение" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Название соревнования:</t>
   </si>
@@ -681,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -770,43 +770,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -817,21 +780,17 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -859,6 +818,43 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA54"/>
+  <dimension ref="A1:Z54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,854 +1339,798 @@
     <col min="3" max="3" width="14.5703125" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="30"/>
-    <col min="12" max="12" width="15.42578125" style="30" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="30"/>
+    <col min="6" max="6" width="20.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="30"/>
+    <col min="11" max="11" width="15.42578125" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-    </row>
-    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="AA2" s="30" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="Z2" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="L3" s="2" t="s">
+    <row r="3" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L4" s="3"/>
-      <c r="M4" s="1" t="s">
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="3"/>
+      <c r="L4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="61" t="s">
+      <c r="F5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="61" t="s">
+      <c r="G5" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="H5" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="68" t="s">
+      <c r="I5" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="1" t="s">
+      <c r="J5" s="31"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31"/>
-      <c r="B6" s="74">
+      <c r="B6" s="57">
         <v>1</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="1" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31"/>
-      <c r="B7" s="73" t="str">
+      <c r="B7" s="56" t="str">
         <f>IF(C7&amp;D7&amp;E7="","",B6+1)</f>
         <v/>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="5" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31"/>
-      <c r="B8" s="73" t="str">
-        <f t="shared" ref="B8:B18" si="0">IF(C8&amp;D8&amp;E8="","",B7+1)</f>
-        <v/>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="5" t="s">
+      <c r="B8" s="56" t="str">
+        <f t="shared" ref="B8:B12" si="0">IF(C8&amp;D8&amp;E8="","",B7+1)</f>
+        <v/>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
-      <c r="B9" s="73" t="str">
+      <c r="B9" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="31"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="34"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="31"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" s="73" t="str">
+      <c r="B10" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="31"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="34"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="31"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" s="73" t="str">
+      <c r="B11" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="31"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="34"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="31"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="73" t="str">
+      <c r="B12" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="34"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="73" t="str">
+      <c r="B13" s="56" t="str">
         <f t="shared" ref="B13:B52" si="1">IF(C13&amp;D13&amp;E13="","",B12+1)</f>
         <v/>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="34"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
-      <c r="B14" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="31"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
-      <c r="B15" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="31"/>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
-      <c r="B16" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="31"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="31"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="31"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="31"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="31"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="31"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
-      <c r="B19" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="31"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="31"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
-      <c r="B20" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="70"/>
-      <c r="K20" s="31"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="31"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
-      <c r="B21" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="31"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="31"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
-      <c r="B22" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="31"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="31"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
-      <c r="B23" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="31"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="31"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
-      <c r="B24" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="31"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="31"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
-      <c r="B25" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="31"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
-      <c r="B26" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="31"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="31"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
-      <c r="B27" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="31"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="70"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="70"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C30" s="47"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="70"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="70"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="70"/>
-    </row>
-    <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="70"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="66"/>
-      <c r="J34" s="70"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="70"/>
-    </row>
-    <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="70"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="70"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="66"/>
-      <c r="J38" s="70"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="70"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="70"/>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="66"/>
-      <c r="J41" s="70"/>
-    </row>
-    <row r="42" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="66"/>
-      <c r="J42" s="70"/>
-    </row>
-    <row r="43" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="70"/>
-    </row>
-    <row r="44" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="70"/>
-    </row>
-    <row r="45" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="66"/>
-      <c r="J45" s="70"/>
-    </row>
-    <row r="46" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="66"/>
-      <c r="J46" s="70"/>
-    </row>
-    <row r="47" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C47" s="47"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="70"/>
-    </row>
-    <row r="48" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C48" s="47"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="70"/>
-    </row>
-    <row r="49" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C49" s="47"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="66"/>
-      <c r="J49" s="70"/>
-    </row>
-    <row r="50" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="70"/>
-    </row>
-    <row r="51" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="70"/>
-    </row>
-    <row r="52" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="73" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="70"/>
-    </row>
-    <row r="53" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="73" t="str">
+      <c r="B27" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="31"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="53"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="53"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="53"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="53"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="53"/>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="53"/>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="53"/>
+    </row>
+    <row r="35" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="53"/>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="53"/>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="53"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C38" s="34"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="53"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C39" s="34"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="53"/>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C40" s="34"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="53"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="53"/>
+    </row>
+    <row r="42" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C42" s="34"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="53"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C43" s="34"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="53"/>
+    </row>
+    <row r="44" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C44" s="34"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="53"/>
+    </row>
+    <row r="45" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C45" s="34"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="53"/>
+    </row>
+    <row r="46" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C46" s="34"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="53"/>
+    </row>
+    <row r="47" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C47" s="34"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="53"/>
+    </row>
+    <row r="48" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C48" s="34"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="53"/>
+    </row>
+    <row r="49" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="53"/>
+    </row>
+    <row r="50" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C50" s="34"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="53"/>
+    </row>
+    <row r="51" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C51" s="34"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="53"/>
+    </row>
+    <row r="52" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C52" s="34"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="53"/>
+    </row>
+    <row r="53" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="56" t="str">
         <f>IF(C53&amp;D53&amp;E53="","",B52+1)</f>
         <v/>
       </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="66"/>
-      <c r="J53" s="71"/>
-    </row>
-    <row r="54" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="75" t="str">
+      <c r="C53" s="34"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="54"/>
+    </row>
+    <row r="54" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="58" t="str">
         <f>IF(C54&amp;D54&amp;E54="","",B53+1)</f>
         <v/>
       </c>
-      <c r="C54" s="48"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="54"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="67"/>
-      <c r="J54" s="72"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:J3"/>
+    <mergeCell ref="B1:I3"/>
   </mergeCells>
-  <conditionalFormatting sqref="L7:L8">
+  <conditionalFormatting sqref="K7:K8">
     <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="✓">
-      <formula>NOT(ISERROR(SEARCH("✓",L7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("✓",K7)))</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="6" priority="2">
-      <formula>LEN(TRIM(L7))&gt;0</formula>
+      <formula>LEN(TRIM(K7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2222,37 +2162,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
     </row>
@@ -2296,11 +2236,11 @@
       <c r="D7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="39" t="str">
+      <c r="E7" s="60" t="str">
         <f>IF(Заполнение!E6="","",Заполнение!E6)</f>
         <v/>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="9"/>
       <c r="H7" s="11"/>
     </row>
@@ -2329,10 +2269,10 @@
       <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="66"/>
       <c r="F10" s="16" t="s">
         <v>6</v>
       </c>
@@ -2351,11 +2291,11 @@
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="D11" s="43" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E11" s="44"/>
+      <c r="D11" s="67" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="68"/>
       <c r="F11" s="20" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2374,14 +2314,14 @@
         <v>#REF!</v>
       </c>
       <c r="C12" s="19" t="str">
-        <f>IF(Заполнение!H5="","",Заполнение!H5)</f>
+        <f>IF(Заполнение!G5="","",Заполнение!G5)</f>
         <v>Регион проживания</v>
       </c>
-      <c r="D12" s="35" t="str">
-        <f>IF(Заполнение!H6="","",Заполнение!H6)</f>
-        <v/>
-      </c>
-      <c r="E12" s="36"/>
+      <c r="D12" s="63" t="str">
+        <f>IF(Заполнение!G6="","",Заполнение!G6)</f>
+        <v/>
+      </c>
+      <c r="E12" s="64"/>
       <c r="F12" s="20" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2401,14 +2341,14 @@
         <v>#REF!</v>
       </c>
       <c r="C13" s="19" t="str">
-        <f>IF(Заполнение!I5="","",Заполнение!I5)</f>
+        <f>IF(Заполнение!H5="","",Заполнение!H5)</f>
         <v>Номер телефона</v>
       </c>
-      <c r="D13" s="35" t="str">
-        <f>IF(Заполнение!I6="","",Заполнение!I6)</f>
-        <v/>
-      </c>
-      <c r="E13" s="36"/>
+      <c r="D13" s="63" t="str">
+        <f>IF(Заполнение!H6="","",Заполнение!H6)</f>
+        <v/>
+      </c>
+      <c r="E13" s="64"/>
       <c r="F13" s="20" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2431,11 +2371,11 @@
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="D14" s="35" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E14" s="36"/>
+      <c r="D14" s="63" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="64"/>
       <c r="F14" s="20" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2458,11 +2398,11 @@
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="D15" s="35" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E15" s="36"/>
+      <c r="D15" s="63" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E15" s="64"/>
       <c r="F15" s="20" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2485,21 +2425,21 @@
         <f>IF(Заполнение!C7="","",Заполнение!C7)</f>
         <v/>
       </c>
-      <c r="D16" s="35" t="str">
+      <c r="D16" s="63" t="str">
         <f>IF(Заполнение!D7="","",Заполнение!D7)</f>
         <v/>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="64"/>
       <c r="F16" s="20" t="str">
         <f>IF(Заполнение!E7="","",Заполнение!E7)</f>
         <v/>
       </c>
-      <c r="G16" s="21" t="str">
+      <c r="G16" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H16" s="18" t="str">
         <f>IF(Заполнение!F7="","",Заполнение!F7)</f>
-        <v/>
-      </c>
-      <c r="H16" s="18" t="str">
-        <f>IF(Заполнение!G7="","",Заполнение!G7)</f>
         <v/>
       </c>
     </row>
@@ -2512,21 +2452,21 @@
         <f>IF(Заполнение!C8="","",Заполнение!C8)</f>
         <v/>
       </c>
-      <c r="D17" s="35" t="str">
+      <c r="D17" s="63" t="str">
         <f>IF(Заполнение!D8="","",Заполнение!D8)</f>
         <v/>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="20" t="str">
         <f>IF(Заполнение!E8="","",Заполнение!E8)</f>
         <v/>
       </c>
-      <c r="G17" s="21" t="str">
+      <c r="G17" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H17" s="18" t="str">
         <f>IF(Заполнение!F8="","",Заполнение!F8)</f>
-        <v/>
-      </c>
-      <c r="H17" s="18" t="str">
-        <f>IF(Заполнение!G8="","",Заполнение!G8)</f>
         <v/>
       </c>
     </row>
@@ -2539,21 +2479,21 @@
         <f>IF(Заполнение!C9="","",Заполнение!C9)</f>
         <v/>
       </c>
-      <c r="D18" s="35" t="str">
+      <c r="D18" s="63" t="str">
         <f>IF(Заполнение!D9="","",Заполнение!D9)</f>
         <v/>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="20" t="str">
         <f>IF(Заполнение!E9="","",Заполнение!E9)</f>
         <v/>
       </c>
-      <c r="G18" s="21" t="str">
+      <c r="G18" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H18" s="18" t="str">
         <f>IF(Заполнение!F9="","",Заполнение!F9)</f>
-        <v/>
-      </c>
-      <c r="H18" s="18" t="str">
-        <f>IF(Заполнение!G9="","",Заполнение!G9)</f>
         <v/>
       </c>
     </row>
@@ -2566,21 +2506,21 @@
         <f>IF(Заполнение!C10="","",Заполнение!C10)</f>
         <v/>
       </c>
-      <c r="D19" s="35" t="str">
+      <c r="D19" s="63" t="str">
         <f>IF(Заполнение!D10="","",Заполнение!D10)</f>
         <v/>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="20" t="str">
         <f>IF(Заполнение!E10="","",Заполнение!E10)</f>
         <v/>
       </c>
-      <c r="G19" s="21" t="str">
+      <c r="G19" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H19" s="18" t="str">
         <f>IF(Заполнение!F10="","",Заполнение!F10)</f>
-        <v/>
-      </c>
-      <c r="H19" s="18" t="str">
-        <f>IF(Заполнение!G10="","",Заполнение!G10)</f>
         <v/>
       </c>
     </row>
@@ -2593,21 +2533,21 @@
         <f>IF(Заполнение!C11="","",Заполнение!C11)</f>
         <v/>
       </c>
-      <c r="D20" s="35" t="str">
+      <c r="D20" s="63" t="str">
         <f>IF(Заполнение!D11="","",Заполнение!D11)</f>
         <v/>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="20" t="str">
         <f>IF(Заполнение!E11="","",Заполнение!E11)</f>
         <v/>
       </c>
-      <c r="G20" s="21" t="str">
+      <c r="G20" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H20" s="18" t="str">
         <f>IF(Заполнение!F11="","",Заполнение!F11)</f>
-        <v/>
-      </c>
-      <c r="H20" s="18" t="str">
-        <f>IF(Заполнение!G11="","",Заполнение!G11)</f>
         <v/>
       </c>
     </row>
@@ -2620,21 +2560,21 @@
         <f>IF(Заполнение!C12="","",Заполнение!C12)</f>
         <v/>
       </c>
-      <c r="D21" s="35" t="str">
+      <c r="D21" s="63" t="str">
         <f>IF(Заполнение!D12="","",Заполнение!D12)</f>
         <v/>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="20" t="str">
         <f>IF(Заполнение!E12="","",Заполнение!E12)</f>
         <v/>
       </c>
-      <c r="G21" s="21" t="str">
+      <c r="G21" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H21" s="18" t="str">
         <f>IF(Заполнение!F12="","",Заполнение!F12)</f>
-        <v/>
-      </c>
-      <c r="H21" s="18" t="str">
-        <f>IF(Заполнение!G12="","",Заполнение!G12)</f>
         <v/>
       </c>
     </row>
@@ -2647,21 +2587,21 @@
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
         <v/>
       </c>
-      <c r="D22" s="35" t="str">
+      <c r="D22" s="63" t="str">
         <f>IF(Заполнение!D13="","",Заполнение!D13)</f>
         <v/>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="64"/>
       <c r="F22" s="20" t="str">
         <f>IF(Заполнение!E13="","",Заполнение!E13)</f>
         <v/>
       </c>
-      <c r="G22" s="21" t="str">
+      <c r="G22" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H22" s="18" t="str">
         <f>IF(Заполнение!F13="","",Заполнение!F13)</f>
-        <v/>
-      </c>
-      <c r="H22" s="18" t="str">
-        <f>IF(Заполнение!G13="","",Заполнение!G13)</f>
         <v/>
       </c>
     </row>
@@ -2674,21 +2614,21 @@
         <f>IF(Заполнение!C50="","",Заполнение!C50)</f>
         <v/>
       </c>
-      <c r="D23" s="35" t="str">
+      <c r="D23" s="63" t="str">
         <f>IF(Заполнение!D50="","",Заполнение!D50)</f>
         <v/>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="64"/>
       <c r="F23" s="20" t="str">
         <f>IF(Заполнение!E50="","",Заполнение!E50)</f>
         <v/>
       </c>
-      <c r="G23" s="21" t="str">
+      <c r="G23" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H23" s="18" t="str">
         <f>IF(Заполнение!F50="","",Заполнение!F50)</f>
-        <v/>
-      </c>
-      <c r="H23" s="18" t="str">
-        <f>IF(Заполнение!G50="","",Заполнение!G50)</f>
         <v/>
       </c>
     </row>
@@ -2701,21 +2641,21 @@
         <f>IF(Заполнение!C51="","",Заполнение!C51)</f>
         <v/>
       </c>
-      <c r="D24" s="35" t="str">
+      <c r="D24" s="63" t="str">
         <f>IF(Заполнение!D51="","",Заполнение!D51)</f>
         <v/>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="20" t="str">
         <f>IF(Заполнение!E51="","",Заполнение!E51)</f>
         <v/>
       </c>
-      <c r="G24" s="21" t="str">
+      <c r="G24" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H24" s="18" t="str">
         <f>IF(Заполнение!F51="","",Заполнение!F51)</f>
-        <v/>
-      </c>
-      <c r="H24" s="18" t="str">
-        <f>IF(Заполнение!G51="","",Заполнение!G51)</f>
         <v/>
       </c>
     </row>
@@ -2728,21 +2668,21 @@
         <f>IF(Заполнение!C52="","",Заполнение!C52)</f>
         <v/>
       </c>
-      <c r="D25" s="35" t="str">
+      <c r="D25" s="63" t="str">
         <f>IF(Заполнение!D52="","",Заполнение!D52)</f>
         <v/>
       </c>
-      <c r="E25" s="36"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="20" t="str">
         <f>IF(Заполнение!E52="","",Заполнение!E52)</f>
         <v/>
       </c>
-      <c r="G25" s="21" t="str">
+      <c r="G25" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H25" s="18" t="str">
         <f>IF(Заполнение!F52="","",Заполнение!F52)</f>
-        <v/>
-      </c>
-      <c r="H25" s="18" t="str">
-        <f>IF(Заполнение!G52="","",Заполнение!G52)</f>
         <v/>
       </c>
     </row>
@@ -2755,21 +2695,21 @@
         <f>IF(Заполнение!C53="","",Заполнение!C53)</f>
         <v/>
       </c>
-      <c r="D26" s="35" t="str">
+      <c r="D26" s="63" t="str">
         <f>IF(Заполнение!D53="","",Заполнение!D53)</f>
         <v/>
       </c>
-      <c r="E26" s="36"/>
+      <c r="E26" s="64"/>
       <c r="F26" s="20" t="str">
         <f>IF(Заполнение!E53="","",Заполнение!E53)</f>
         <v/>
       </c>
-      <c r="G26" s="21" t="str">
+      <c r="G26" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H26" s="18" t="str">
         <f>IF(Заполнение!F53="","",Заполнение!F53)</f>
-        <v/>
-      </c>
-      <c r="H26" s="18" t="str">
-        <f>IF(Заполнение!G53="","",Заполнение!G53)</f>
         <v/>
       </c>
     </row>
@@ -2782,21 +2722,21 @@
         <f>IF(Заполнение!C54="","",Заполнение!C54)</f>
         <v/>
       </c>
-      <c r="D27" s="35" t="str">
+      <c r="D27" s="63" t="str">
         <f>IF(Заполнение!D54="","",Заполнение!D54)</f>
         <v/>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="20" t="str">
         <f>IF(Заполнение!E54="","",Заполнение!E54)</f>
         <v/>
       </c>
-      <c r="G27" s="21" t="str">
+      <c r="G27" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H27" s="18" t="str">
         <f>IF(Заполнение!F54="","",Заполнение!F54)</f>
-        <v/>
-      </c>
-      <c r="H27" s="18" t="str">
-        <f>IF(Заполнение!G54="","",Заполнение!G54)</f>
         <v/>
       </c>
     </row>
@@ -2809,21 +2749,21 @@
         <f>IF(Заполнение!C30="","",Заполнение!C30)</f>
         <v/>
       </c>
-      <c r="D28" s="35" t="str">
+      <c r="D28" s="63" t="str">
         <f>IF(Заполнение!D30="","",Заполнение!D30)</f>
         <v/>
       </c>
-      <c r="E28" s="36"/>
+      <c r="E28" s="64"/>
       <c r="F28" s="20" t="str">
         <f>IF(Заполнение!E30="","",Заполнение!E30)</f>
         <v/>
       </c>
-      <c r="G28" s="21" t="str">
+      <c r="G28" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H28" s="18" t="str">
         <f>IF(Заполнение!F30="","",Заполнение!F30)</f>
-        <v/>
-      </c>
-      <c r="H28" s="18" t="str">
-        <f>IF(Заполнение!G30="","",Заполнение!G30)</f>
         <v/>
       </c>
     </row>
@@ -2836,21 +2776,21 @@
         <f>IF(Заполнение!C31="","",Заполнение!C31)</f>
         <v/>
       </c>
-      <c r="D29" s="35" t="str">
+      <c r="D29" s="63" t="str">
         <f>IF(Заполнение!D31="","",Заполнение!D31)</f>
         <v/>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="64"/>
       <c r="F29" s="20" t="str">
         <f>IF(Заполнение!E31="","",Заполнение!E31)</f>
         <v/>
       </c>
-      <c r="G29" s="21" t="str">
+      <c r="G29" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H29" s="18" t="str">
         <f>IF(Заполнение!F31="","",Заполнение!F31)</f>
-        <v/>
-      </c>
-      <c r="H29" s="18" t="str">
-        <f>IF(Заполнение!G31="","",Заполнение!G31)</f>
         <v/>
       </c>
     </row>
@@ -2863,21 +2803,21 @@
         <f>IF(Заполнение!C32="","",Заполнение!C32)</f>
         <v/>
       </c>
-      <c r="D30" s="35" t="str">
+      <c r="D30" s="63" t="str">
         <f>IF(Заполнение!D32="","",Заполнение!D32)</f>
         <v/>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="20" t="str">
         <f>IF(Заполнение!E32="","",Заполнение!E32)</f>
         <v/>
       </c>
-      <c r="G30" s="21" t="str">
+      <c r="G30" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H30" s="18" t="str">
         <f>IF(Заполнение!F32="","",Заполнение!F32)</f>
-        <v/>
-      </c>
-      <c r="H30" s="18" t="str">
-        <f>IF(Заполнение!G32="","",Заполнение!G32)</f>
         <v/>
       </c>
     </row>
@@ -2890,21 +2830,21 @@
         <f>IF(Заполнение!C33="","",Заполнение!C33)</f>
         <v/>
       </c>
-      <c r="D31" s="35" t="str">
+      <c r="D31" s="63" t="str">
         <f>IF(Заполнение!D33="","",Заполнение!D33)</f>
         <v/>
       </c>
-      <c r="E31" s="36"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="20" t="str">
         <f>IF(Заполнение!E33="","",Заполнение!E33)</f>
         <v/>
       </c>
-      <c r="G31" s="21" t="str">
+      <c r="G31" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H31" s="18" t="str">
         <f>IF(Заполнение!F33="","",Заполнение!F33)</f>
-        <v/>
-      </c>
-      <c r="H31" s="18" t="str">
-        <f>IF(Заполнение!G33="","",Заполнение!G33)</f>
         <v/>
       </c>
     </row>
@@ -2917,21 +2857,21 @@
         <f>IF(Заполнение!C34="","",Заполнение!C34)</f>
         <v/>
       </c>
-      <c r="D32" s="35" t="str">
+      <c r="D32" s="63" t="str">
         <f>IF(Заполнение!D34="","",Заполнение!D34)</f>
         <v/>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="20" t="str">
         <f>IF(Заполнение!E34="","",Заполнение!E34)</f>
         <v/>
       </c>
-      <c r="G32" s="21" t="str">
+      <c r="G32" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H32" s="18" t="str">
         <f>IF(Заполнение!F34="","",Заполнение!F34)</f>
-        <v/>
-      </c>
-      <c r="H32" s="18" t="str">
-        <f>IF(Заполнение!G34="","",Заполнение!G34)</f>
         <v/>
       </c>
     </row>
@@ -2944,21 +2884,21 @@
         <f>IF(Заполнение!C35="","",Заполнение!C35)</f>
         <v/>
       </c>
-      <c r="D33" s="35" t="str">
+      <c r="D33" s="63" t="str">
         <f>IF(Заполнение!D35="","",Заполнение!D35)</f>
         <v/>
       </c>
-      <c r="E33" s="36"/>
+      <c r="E33" s="64"/>
       <c r="F33" s="20" t="str">
         <f>IF(Заполнение!E35="","",Заполнение!E35)</f>
         <v/>
       </c>
-      <c r="G33" s="21" t="str">
+      <c r="G33" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H33" s="18" t="str">
         <f>IF(Заполнение!F35="","",Заполнение!F35)</f>
-        <v/>
-      </c>
-      <c r="H33" s="18" t="str">
-        <f>IF(Заполнение!G35="","",Заполнение!G35)</f>
         <v/>
       </c>
     </row>
@@ -2971,21 +2911,21 @@
         <f>IF(Заполнение!C36="","",Заполнение!C36)</f>
         <v/>
       </c>
-      <c r="D34" s="35" t="str">
+      <c r="D34" s="63" t="str">
         <f>IF(Заполнение!D36="","",Заполнение!D36)</f>
         <v/>
       </c>
-      <c r="E34" s="36"/>
+      <c r="E34" s="64"/>
       <c r="F34" s="20" t="str">
         <f>IF(Заполнение!E36="","",Заполнение!E36)</f>
         <v/>
       </c>
-      <c r="G34" s="21" t="str">
+      <c r="G34" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H34" s="18" t="str">
         <f>IF(Заполнение!F36="","",Заполнение!F36)</f>
-        <v/>
-      </c>
-      <c r="H34" s="18" t="str">
-        <f>IF(Заполнение!G36="","",Заполнение!G36)</f>
         <v/>
       </c>
     </row>
@@ -2998,21 +2938,21 @@
         <f>IF(Заполнение!C37="","",Заполнение!C37)</f>
         <v/>
       </c>
-      <c r="D35" s="35" t="str">
+      <c r="D35" s="63" t="str">
         <f>IF(Заполнение!D37="","",Заполнение!D37)</f>
         <v/>
       </c>
-      <c r="E35" s="36"/>
+      <c r="E35" s="64"/>
       <c r="F35" s="20" t="str">
         <f>IF(Заполнение!E37="","",Заполнение!E37)</f>
         <v/>
       </c>
-      <c r="G35" s="21" t="str">
+      <c r="G35" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H35" s="18" t="str">
         <f>IF(Заполнение!F37="","",Заполнение!F37)</f>
-        <v/>
-      </c>
-      <c r="H35" s="18" t="str">
-        <f>IF(Заполнение!G37="","",Заполнение!G37)</f>
         <v/>
       </c>
     </row>
@@ -3025,21 +2965,21 @@
         <f>IF(Заполнение!C38="","",Заполнение!C38)</f>
         <v/>
       </c>
-      <c r="D36" s="35" t="str">
+      <c r="D36" s="63" t="str">
         <f>IF(Заполнение!D38="","",Заполнение!D38)</f>
         <v/>
       </c>
-      <c r="E36" s="36"/>
+      <c r="E36" s="64"/>
       <c r="F36" s="20" t="str">
         <f>IF(Заполнение!E38="","",Заполнение!E38)</f>
         <v/>
       </c>
-      <c r="G36" s="21" t="str">
+      <c r="G36" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H36" s="18" t="str">
         <f>IF(Заполнение!F38="","",Заполнение!F38)</f>
-        <v/>
-      </c>
-      <c r="H36" s="18" t="str">
-        <f>IF(Заполнение!G38="","",Заполнение!G38)</f>
         <v/>
       </c>
     </row>
@@ -3052,21 +2992,21 @@
         <f>IF(Заполнение!C39="","",Заполнение!C39)</f>
         <v/>
       </c>
-      <c r="D37" s="35" t="str">
+      <c r="D37" s="63" t="str">
         <f>IF(Заполнение!D39="","",Заполнение!D39)</f>
         <v/>
       </c>
-      <c r="E37" s="36"/>
+      <c r="E37" s="64"/>
       <c r="F37" s="20" t="str">
         <f>IF(Заполнение!E39="","",Заполнение!E39)</f>
         <v/>
       </c>
-      <c r="G37" s="21" t="str">
+      <c r="G37" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H37" s="18" t="str">
         <f>IF(Заполнение!F39="","",Заполнение!F39)</f>
-        <v/>
-      </c>
-      <c r="H37" s="18" t="str">
-        <f>IF(Заполнение!G39="","",Заполнение!G39)</f>
         <v/>
       </c>
     </row>
@@ -3079,21 +3019,21 @@
         <f>IF(Заполнение!C40="","",Заполнение!C40)</f>
         <v/>
       </c>
-      <c r="D38" s="35" t="str">
+      <c r="D38" s="63" t="str">
         <f>IF(Заполнение!D40="","",Заполнение!D40)</f>
         <v/>
       </c>
-      <c r="E38" s="36"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="20" t="str">
         <f>IF(Заполнение!E40="","",Заполнение!E40)</f>
         <v/>
       </c>
-      <c r="G38" s="21" t="str">
+      <c r="G38" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H38" s="18" t="str">
         <f>IF(Заполнение!F40="","",Заполнение!F40)</f>
-        <v/>
-      </c>
-      <c r="H38" s="18" t="str">
-        <f>IF(Заполнение!G40="","",Заполнение!G40)</f>
         <v/>
       </c>
     </row>
@@ -3106,21 +3046,21 @@
         <f>IF(Заполнение!C41="","",Заполнение!C41)</f>
         <v/>
       </c>
-      <c r="D39" s="35" t="str">
+      <c r="D39" s="63" t="str">
         <f>IF(Заполнение!D41="","",Заполнение!D41)</f>
         <v/>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="20" t="str">
         <f>IF(Заполнение!E41="","",Заполнение!E41)</f>
         <v/>
       </c>
-      <c r="G39" s="21" t="str">
+      <c r="G39" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H39" s="18" t="str">
         <f>IF(Заполнение!F41="","",Заполнение!F41)</f>
-        <v/>
-      </c>
-      <c r="H39" s="18" t="str">
-        <f>IF(Заполнение!G41="","",Заполнение!G41)</f>
         <v/>
       </c>
     </row>
@@ -3133,21 +3073,21 @@
         <f>IF(Заполнение!C42="","",Заполнение!C42)</f>
         <v/>
       </c>
-      <c r="D40" s="35" t="str">
+      <c r="D40" s="63" t="str">
         <f>IF(Заполнение!D42="","",Заполнение!D42)</f>
         <v/>
       </c>
-      <c r="E40" s="36"/>
+      <c r="E40" s="64"/>
       <c r="F40" s="20" t="str">
         <f>IF(Заполнение!E42="","",Заполнение!E42)</f>
         <v/>
       </c>
-      <c r="G40" s="21" t="str">
+      <c r="G40" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H40" s="18" t="str">
         <f>IF(Заполнение!F42="","",Заполнение!F42)</f>
-        <v/>
-      </c>
-      <c r="H40" s="18" t="str">
-        <f>IF(Заполнение!G42="","",Заполнение!G42)</f>
         <v/>
       </c>
     </row>
@@ -3160,21 +3100,21 @@
         <f>IF(Заполнение!C43="","",Заполнение!C43)</f>
         <v/>
       </c>
-      <c r="D41" s="35" t="str">
+      <c r="D41" s="63" t="str">
         <f>IF(Заполнение!D43="","",Заполнение!D43)</f>
         <v/>
       </c>
-      <c r="E41" s="36"/>
+      <c r="E41" s="64"/>
       <c r="F41" s="20" t="str">
         <f>IF(Заполнение!E43="","",Заполнение!E43)</f>
         <v/>
       </c>
-      <c r="G41" s="21" t="str">
+      <c r="G41" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H41" s="18" t="str">
         <f>IF(Заполнение!F43="","",Заполнение!F43)</f>
-        <v/>
-      </c>
-      <c r="H41" s="18" t="str">
-        <f>IF(Заполнение!G43="","",Заполнение!G43)</f>
         <v/>
       </c>
     </row>
@@ -3187,21 +3127,21 @@
         <f>IF(Заполнение!C44="","",Заполнение!C44)</f>
         <v/>
       </c>
-      <c r="D42" s="35" t="str">
+      <c r="D42" s="63" t="str">
         <f>IF(Заполнение!D44="","",Заполнение!D44)</f>
         <v/>
       </c>
-      <c r="E42" s="36"/>
+      <c r="E42" s="64"/>
       <c r="F42" s="20" t="str">
         <f>IF(Заполнение!E44="","",Заполнение!E44)</f>
         <v/>
       </c>
-      <c r="G42" s="21" t="str">
+      <c r="G42" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H42" s="18" t="str">
         <f>IF(Заполнение!F44="","",Заполнение!F44)</f>
-        <v/>
-      </c>
-      <c r="H42" s="18" t="str">
-        <f>IF(Заполнение!G44="","",Заполнение!G44)</f>
         <v/>
       </c>
     </row>
@@ -3214,21 +3154,21 @@
         <f>IF(Заполнение!C45="","",Заполнение!C45)</f>
         <v/>
       </c>
-      <c r="D43" s="35" t="str">
+      <c r="D43" s="63" t="str">
         <f>IF(Заполнение!D45="","",Заполнение!D45)</f>
         <v/>
       </c>
-      <c r="E43" s="36"/>
+      <c r="E43" s="64"/>
       <c r="F43" s="20" t="str">
         <f>IF(Заполнение!E45="","",Заполнение!E45)</f>
         <v/>
       </c>
-      <c r="G43" s="21" t="str">
+      <c r="G43" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H43" s="18" t="str">
         <f>IF(Заполнение!F45="","",Заполнение!F45)</f>
-        <v/>
-      </c>
-      <c r="H43" s="18" t="str">
-        <f>IF(Заполнение!G45="","",Заполнение!G45)</f>
         <v/>
       </c>
     </row>
@@ -3241,21 +3181,21 @@
         <f>IF(Заполнение!C46="","",Заполнение!C46)</f>
         <v/>
       </c>
-      <c r="D44" s="35" t="str">
+      <c r="D44" s="63" t="str">
         <f>IF(Заполнение!D46="","",Заполнение!D46)</f>
         <v/>
       </c>
-      <c r="E44" s="36"/>
+      <c r="E44" s="64"/>
       <c r="F44" s="20" t="str">
         <f>IF(Заполнение!E46="","",Заполнение!E46)</f>
         <v/>
       </c>
-      <c r="G44" s="21" t="str">
+      <c r="G44" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H44" s="18" t="str">
         <f>IF(Заполнение!F46="","",Заполнение!F46)</f>
-        <v/>
-      </c>
-      <c r="H44" s="18" t="str">
-        <f>IF(Заполнение!G46="","",Заполнение!G46)</f>
         <v/>
       </c>
     </row>
@@ -3268,21 +3208,21 @@
         <f>IF(Заполнение!C47="","",Заполнение!C47)</f>
         <v/>
       </c>
-      <c r="D45" s="35" t="str">
+      <c r="D45" s="63" t="str">
         <f>IF(Заполнение!D47="","",Заполнение!D47)</f>
         <v/>
       </c>
-      <c r="E45" s="36"/>
+      <c r="E45" s="64"/>
       <c r="F45" s="20" t="str">
         <f>IF(Заполнение!E47="","",Заполнение!E47)</f>
         <v/>
       </c>
-      <c r="G45" s="21" t="str">
+      <c r="G45" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H45" s="18" t="str">
         <f>IF(Заполнение!F47="","",Заполнение!F47)</f>
-        <v/>
-      </c>
-      <c r="H45" s="18" t="str">
-        <f>IF(Заполнение!G47="","",Заполнение!G47)</f>
         <v/>
       </c>
     </row>
@@ -3295,21 +3235,21 @@
         <f>IF(Заполнение!C48="","",Заполнение!C48)</f>
         <v/>
       </c>
-      <c r="D46" s="35" t="str">
+      <c r="D46" s="63" t="str">
         <f>IF(Заполнение!D48="","",Заполнение!D48)</f>
         <v/>
       </c>
-      <c r="E46" s="36"/>
+      <c r="E46" s="64"/>
       <c r="F46" s="20" t="str">
         <f>IF(Заполнение!E48="","",Заполнение!E48)</f>
         <v/>
       </c>
-      <c r="G46" s="21" t="str">
+      <c r="G46" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H46" s="18" t="str">
         <f>IF(Заполнение!F48="","",Заполнение!F48)</f>
-        <v/>
-      </c>
-      <c r="H46" s="18" t="str">
-        <f>IF(Заполнение!G48="","",Заполнение!G48)</f>
         <v/>
       </c>
     </row>
@@ -3322,21 +3262,21 @@
         <f>IF(Заполнение!C49="","",Заполнение!C49)</f>
         <v/>
       </c>
-      <c r="D47" s="35" t="str">
+      <c r="D47" s="63" t="str">
         <f>IF(Заполнение!D49="","",Заполнение!D49)</f>
         <v/>
       </c>
-      <c r="E47" s="36"/>
+      <c r="E47" s="64"/>
       <c r="F47" s="20" t="str">
         <f>IF(Заполнение!E49="","",Заполнение!E49)</f>
         <v/>
       </c>
-      <c r="G47" s="21" t="str">
+      <c r="G47" s="21" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H47" s="18" t="str">
         <f>IF(Заполнение!F49="","",Заполнение!F49)</f>
-        <v/>
-      </c>
-      <c r="H47" s="18" t="str">
-        <f>IF(Заполнение!G49="","",Заполнение!G49)</f>
         <v/>
       </c>
     </row>
@@ -3349,11 +3289,11 @@
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="D48" s="35" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E48" s="36"/>
+      <c r="D48" s="63" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E48" s="64"/>
       <c r="F48" s="20" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3376,11 +3316,11 @@
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="D49" s="37" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E49" s="38"/>
+      <c r="D49" s="69" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E49" s="70"/>
       <c r="F49" s="24" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3395,305 +3335,305 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
       <c r="H50" s="8"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="33" t="s">
+      <c r="B52" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="40" t="s">
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="H52" s="40"/>
+      <c r="H52" s="62"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="40" t="s">
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="H53" s="40"/>
+      <c r="H53" s="62"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="40" t="s">
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="40"/>
+      <c r="H54" s="62"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
       <c r="H57" s="8"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
       <c r="H59" s="8"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="61"/>
       <c r="H63" s="8"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
       <c r="H64" s="8"/>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="61"/>
       <c r="H65" s="8"/>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="33"/>
-      <c r="E66" s="33"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="61"/>
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D67" s="33"/>
-      <c r="E67" s="33"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="61"/>
       <c r="H67" s="8"/>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D68" s="33"/>
-      <c r="E68" s="33"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="61"/>
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="61"/>
       <c r="H69" s="8"/>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
+      <c r="D70" s="61"/>
+      <c r="E70" s="61"/>
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="33"/>
-      <c r="E71" s="33"/>
+      <c r="D71" s="61"/>
+      <c r="E71" s="61"/>
       <c r="H71" s="8"/>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="33"/>
-      <c r="E72" s="33"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
       <c r="H72" s="8"/>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="33"/>
-      <c r="E73" s="33"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="61"/>
       <c r="H73" s="8"/>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="33"/>
-      <c r="E74" s="33"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="61"/>
       <c r="H74" s="8"/>
     </row>
     <row r="75" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
       <c r="H75" s="8"/>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="61"/>
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61"/>
       <c r="H77" s="8"/>
     </row>
     <row r="78" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
+      <c r="D78" s="61"/>
+      <c r="E78" s="61"/>
       <c r="H78" s="8"/>
     </row>
     <row r="79" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
       <c r="H80" s="8"/>
     </row>
     <row r="81" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
       <c r="H81" s="8"/>
     </row>
     <row r="82" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="61"/>
       <c r="H82" s="8"/>
     </row>
     <row r="83" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D84" s="33"/>
-      <c r="E84" s="33"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="61"/>
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="33"/>
-      <c r="E85" s="33"/>
+      <c r="D85" s="61"/>
+      <c r="E85" s="61"/>
       <c r="H85" s="8"/>
     </row>
     <row r="86" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D86" s="33"/>
-      <c r="E86" s="33"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="61"/>
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D87" s="33"/>
-      <c r="E87" s="33"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="61"/>
       <c r="H87" s="8"/>
     </row>
     <row r="88" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="61"/>
       <c r="H88" s="8"/>
     </row>
     <row r="89" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D89" s="33"/>
-      <c r="E89" s="33"/>
+      <c r="D89" s="61"/>
+      <c r="E89" s="61"/>
       <c r="H89" s="8"/>
     </row>
     <row r="90" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D91" s="33"/>
-      <c r="E91" s="33"/>
+      <c r="D91" s="61"/>
+      <c r="E91" s="61"/>
       <c r="H91" s="8"/>
     </row>
     <row r="92" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D92" s="33"/>
-      <c r="E92" s="33"/>
+      <c r="D92" s="61"/>
+      <c r="E92" s="61"/>
       <c r="H92" s="8"/>
     </row>
     <row r="93" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D93" s="33"/>
-      <c r="E93" s="33"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="61"/>
       <c r="H93" s="8"/>
     </row>
     <row r="94" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
       <c r="H94" s="8"/>
     </row>
     <row r="95" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="33"/>
-      <c r="E95" s="33"/>
+      <c r="D95" s="61"/>
+      <c r="E95" s="61"/>
       <c r="H95" s="8"/>
     </row>
     <row r="96" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="33"/>
-      <c r="E96" s="33"/>
+      <c r="D96" s="61"/>
+      <c r="E96" s="61"/>
       <c r="H96" s="8"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D97" s="33"/>
-      <c r="E97" s="33"/>
+      <c r="D97" s="61"/>
+      <c r="E97" s="61"/>
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="33"/>
-      <c r="E98" s="33"/>
+      <c r="D98" s="61"/>
+      <c r="E98" s="61"/>
       <c r="H98" s="8"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D99" s="33"/>
-      <c r="E99" s="33"/>
+      <c r="D99" s="61"/>
+      <c r="E99" s="61"/>
       <c r="H99" s="8"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D100" s="33"/>
-      <c r="E100" s="33"/>
+      <c r="D100" s="61"/>
+      <c r="E100" s="61"/>
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D101" s="33"/>
-      <c r="E101" s="33"/>
+      <c r="D101" s="61"/>
+      <c r="E101" s="61"/>
       <c r="H101" s="8"/>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D102" s="33"/>
-      <c r="E102" s="33"/>
+      <c r="D102" s="61"/>
+      <c r="E102" s="61"/>
       <c r="H102" s="8"/>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D103" s="33"/>
-      <c r="E103" s="33"/>
+      <c r="D103" s="61"/>
+      <c r="E103" s="61"/>
       <c r="H103" s="8"/>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D104" s="33"/>
-      <c r="E104" s="33"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="61"/>
       <c r="H104" s="8"/>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D105" s="33"/>
-      <c r="E105" s="33"/>
+      <c r="D105" s="61"/>
+      <c r="E105" s="61"/>
       <c r="H105" s="8"/>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D106" s="33"/>
-      <c r="E106" s="33"/>
+      <c r="D106" s="61"/>
+      <c r="E106" s="61"/>
       <c r="H106" s="8"/>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D107" s="33"/>
-      <c r="E107" s="33"/>
+      <c r="D107" s="61"/>
+      <c r="E107" s="61"/>
       <c r="H107" s="8"/>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D108" s="33"/>
-      <c r="E108" s="33"/>
+      <c r="D108" s="61"/>
+      <c r="E108" s="61"/>
       <c r="H108" s="8"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D109" s="33"/>
-      <c r="E109" s="33"/>
+      <c r="D109" s="61"/>
+      <c r="E109" s="61"/>
       <c r="H109" s="8"/>
     </row>
     <row r="111" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3709,6 +3649,83 @@
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="B1:H3"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B54:F54"/>
     <mergeCell ref="B52:F52"/>
@@ -3733,83 +3750,6 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="B1:H3"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D83:E83"/>
   </mergeCells>
   <conditionalFormatting sqref="J11:J109">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="✓">

</xml_diff>

<commit_message>
feat: add list of referees to second sheet of New Competition template, Improve Excel files moderation
</commit_message>
<xml_diff>
--- a/Resources/Template_Referee.xlsx
+++ b/Resources/Template_Referee.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Femida_v3\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Femida_v3\Resources\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1602F2D0-5051-41BC-941B-42884628E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D685A6-9F34-4217-B20C-4CC7578697F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заполнение" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>№</t>
   </si>
@@ -153,6 +153,12 @@
     <t>Существующие судьи</t>
   </si>
   <si>
+    <t>Фамилия</t>
+  </si>
+  <si>
+    <t>Проверка</t>
+  </si>
+  <si>
     <t>Саяфаров</t>
   </si>
   <si>
@@ -162,6 +168,9 @@
     <t>Сабирьянович</t>
   </si>
   <si>
+    <t>Саяфаров Валерий Сабирьянович</t>
+  </si>
+  <si>
     <t>Ершов</t>
   </si>
   <si>
@@ -171,6 +180,9 @@
     <t>Валентинович</t>
   </si>
   <si>
+    <t>Ершов Александр Валентинович</t>
+  </si>
+  <si>
     <t>Марченко</t>
   </si>
   <si>
@@ -180,24 +192,36 @@
     <t>Анатольевич</t>
   </si>
   <si>
+    <t>Марченко Юрий Анатольевич</t>
+  </si>
+  <si>
     <t>Соловьев</t>
   </si>
   <si>
     <t>Вячеславович</t>
   </si>
   <si>
+    <t>Соловьев Александр Вячеславович</t>
+  </si>
+  <si>
     <t>Панаков</t>
   </si>
   <si>
     <t>Дивлохович</t>
   </si>
   <si>
+    <t>Панаков Александр Дивлохович</t>
+  </si>
+  <si>
     <t>Ушаков</t>
   </si>
   <si>
     <t>Евгеньевич</t>
   </si>
   <si>
+    <t>Ушаков Александр Евгеньевич</t>
+  </si>
+  <si>
     <t>Духов</t>
   </si>
   <si>
@@ -207,6 +231,9 @@
     <t>Валерьевич</t>
   </si>
   <si>
+    <t>Духов Михаил Валерьевич</t>
+  </si>
+  <si>
     <t>Алексанов</t>
   </si>
   <si>
@@ -216,13 +243,28 @@
     <t>Николаевич</t>
   </si>
   <si>
+    <t>Алексанов Андрей Николаевич</t>
+  </si>
+  <si>
     <t>Пролубников</t>
   </si>
   <si>
     <t>Олег</t>
   </si>
   <si>
-    <t>Фамилия</t>
+    <t>Пролубников Олег Николаевич</t>
+  </si>
+  <si>
+    <t>Битук</t>
+  </si>
+  <si>
+    <t>Евгений</t>
+  </si>
+  <si>
+    <t>Иванович</t>
+  </si>
+  <si>
+    <t>Битук Евгений Иванович</t>
   </si>
 </sst>
 </file>
@@ -704,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -869,6 +911,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1257,67 +1306,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="4.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.42578125" style="18" customWidth="1"/>
-    <col min="11" max="11" width="22" style="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="8"/>
-    <col min="13" max="13" width="15.42578125" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" style="8" width="9.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="4.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="8" width="18.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="13.5703125"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" style="8" width="20.42578125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="29.140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="18" width="14.42578125"/>
+    <col min="9" max="10" customWidth="true" style="18" width="14.42578125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="48" width="22.0"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="64" width="20.42578125"/>
+    <col min="13" max="13" customWidth="true" style="8" width="15.42578125"/>
+    <col min="14" max="16384" style="8" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
     </row>
     <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
       <c r="AB2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1355,7 +1401,9 @@
       <c r="K5" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="65" t="s">
+        <v>21</v>
+      </c>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -1372,7 +1420,10 @@
       <c r="I6" s="53"/>
       <c r="J6" s="53"/>
       <c r="K6" s="54"/>
-      <c r="L6" s="9"/>
+      <c r="L6" s="66" t="str">
+        <f><![CDATA[IF(AND(B6<>"",C6<>""),IF(IFERROR(MATCH(C6&" "&D6&" "&E6,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -1390,7 +1441,10 @@
       <c r="I7" s="53"/>
       <c r="J7" s="53"/>
       <c r="K7" s="54"/>
-      <c r="L7" s="9"/>
+      <c r="L7" s="66" t="str">
+        <f><![CDATA[IF(AND(B7<>"",C7<>""),IF(IFERROR(MATCH(C7&" "&D7&" "&E7,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
@@ -1407,7 +1461,10 @@
       <c r="I8" s="53"/>
       <c r="J8" s="53"/>
       <c r="K8" s="54"/>
-      <c r="L8" s="9"/>
+      <c r="L8" s="66" t="str">
+        <f><![CDATA[IF(AND(B8<>"",C8<>""),IF(IFERROR(MATCH(C8&" "&D8&" "&E8,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -1424,7 +1481,10 @@
       <c r="I9" s="53"/>
       <c r="J9" s="53"/>
       <c r="K9" s="54"/>
-      <c r="L9" s="9"/>
+      <c r="L9" s="66" t="str">
+        <f><![CDATA[IF(AND(B9<>"",C9<>""),IF(IFERROR(MATCH(C9&" "&D9&" "&E9,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
@@ -1441,7 +1501,10 @@
       <c r="I10" s="53"/>
       <c r="J10" s="53"/>
       <c r="K10" s="54"/>
-      <c r="L10" s="9"/>
+      <c r="L10" s="66" t="str">
+        <f><![CDATA[IF(AND(B10<>"",C10<>""),IF(IFERROR(MATCH(C10&" "&D10&" "&E10,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
@@ -1458,7 +1521,10 @@
       <c r="I11" s="53"/>
       <c r="J11" s="53"/>
       <c r="K11" s="54"/>
-      <c r="L11" s="9"/>
+      <c r="L11" s="66" t="str">
+        <f><![CDATA[IF(AND(B11<>"",C11<>""),IF(IFERROR(MATCH(C11&" "&D11&" "&E11,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1475,7 +1541,10 @@
       <c r="I12" s="53"/>
       <c r="J12" s="53"/>
       <c r="K12" s="54"/>
-      <c r="L12" s="9"/>
+      <c r="L12" s="66" t="str">
+        <f><![CDATA[IF(AND(B12<>"",C12<>""),IF(IFERROR(MATCH(C12&" "&D12&" "&E12,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
@@ -1492,7 +1561,10 @@
       <c r="I13" s="53"/>
       <c r="J13" s="53"/>
       <c r="K13" s="54"/>
-      <c r="L13" s="9"/>
+      <c r="L13" s="66" t="str">
+        <f><![CDATA[IF(AND(B13<>"",C13<>""),IF(IFERROR(MATCH(C13&" "&D13&" "&E13,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
@@ -1509,7 +1581,10 @@
       <c r="I14" s="53"/>
       <c r="J14" s="53"/>
       <c r="K14" s="54"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="66" t="str">
+        <f><![CDATA[IF(AND(B14<>"",C14<>""),IF(IFERROR(MATCH(C14&" "&D14&" "&E14,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1526,7 +1601,10 @@
       <c r="I15" s="53"/>
       <c r="J15" s="53"/>
       <c r="K15" s="54"/>
-      <c r="L15" s="9"/>
+      <c r="L15" s="66" t="str">
+        <f><![CDATA[IF(AND(B15<>"",C15<>""),IF(IFERROR(MATCH(C15&" "&D15&" "&E15,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1543,7 +1621,10 @@
       <c r="I16" s="53"/>
       <c r="J16" s="53"/>
       <c r="K16" s="54"/>
-      <c r="L16" s="9"/>
+      <c r="L16" s="66" t="str">
+        <f><![CDATA[IF(AND(B16<>"",C16<>""),IF(IFERROR(MATCH(C16&" "&D16&" "&E16,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1560,7 +1641,10 @@
       <c r="I17" s="53"/>
       <c r="J17" s="53"/>
       <c r="K17" s="54"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="66" t="str">
+        <f><![CDATA[IF(AND(B17<>"",C17<>""),IF(IFERROR(MATCH(C17&" "&D17&" "&E17,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1577,7 +1661,10 @@
       <c r="I18" s="53"/>
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="9"/>
+      <c r="L18" s="66" t="str">
+        <f><![CDATA[IF(AND(B18<>"",C18<>""),IF(IFERROR(MATCH(C18&" "&D18&" "&E18,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1594,7 +1681,10 @@
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
       <c r="K19" s="54"/>
-      <c r="L19" s="9"/>
+      <c r="L19" s="66" t="str">
+        <f><![CDATA[IF(AND(B19<>"",C19<>""),IF(IFERROR(MATCH(C19&" "&D19&" "&E19,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1611,7 +1701,10 @@
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
       <c r="K20" s="54"/>
-      <c r="L20" s="9"/>
+      <c r="L20" s="66" t="str">
+        <f><![CDATA[IF(AND(B20<>"",C20<>""),IF(IFERROR(MATCH(C20&" "&D20&" "&E20,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1628,7 +1721,10 @@
       <c r="I21" s="53"/>
       <c r="J21" s="53"/>
       <c r="K21" s="54"/>
-      <c r="L21" s="9"/>
+      <c r="L21" s="66" t="str">
+        <f><![CDATA[IF(AND(B21<>"",C21<>""),IF(IFERROR(MATCH(C21&" "&D21&" "&E21,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1645,7 +1741,10 @@
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
       <c r="K22" s="54"/>
-      <c r="L22" s="9"/>
+      <c r="L22" s="66" t="str">
+        <f><![CDATA[IF(AND(B22<>"",C22<>""),IF(IFERROR(MATCH(C22&" "&D22&" "&E22,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1662,7 +1761,10 @@
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
       <c r="K23" s="54"/>
-      <c r="L23" s="9"/>
+      <c r="L23" s="66" t="str">
+        <f><![CDATA[IF(AND(B23<>"",C23<>""),IF(IFERROR(MATCH(C23&" "&D23&" "&E23,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1679,7 +1781,10 @@
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
       <c r="K24" s="54"/>
-      <c r="L24" s="9"/>
+      <c r="L24" s="66" t="str">
+        <f><![CDATA[IF(AND(B24<>"",C24<>""),IF(IFERROR(MATCH(C24&" "&D24&" "&E24,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1696,7 +1801,10 @@
       <c r="I25" s="53"/>
       <c r="J25" s="53"/>
       <c r="K25" s="54"/>
-      <c r="L25" s="9"/>
+      <c r="L25" s="66" t="str">
+        <f><![CDATA[IF(AND(B25<>"",C25<>""),IF(IFERROR(MATCH(C25&" "&D25&" "&E25,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1713,7 +1821,10 @@
       <c r="I26" s="53"/>
       <c r="J26" s="53"/>
       <c r="K26" s="54"/>
-      <c r="L26" s="9"/>
+      <c r="L26" s="66" t="str">
+        <f><![CDATA[IF(AND(B26<>"",C26<>""),IF(IFERROR(MATCH(C26&" "&D26&" "&E26,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1730,7 +1841,10 @@
       <c r="I27" s="53"/>
       <c r="J27" s="53"/>
       <c r="K27" s="54"/>
-      <c r="L27" s="9"/>
+      <c r="L27" s="66" t="str">
+        <f><![CDATA[IF(AND(B27<>"",C27<>""),IF(IFERROR(MATCH(C27&" "&D27&" "&E27,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="61" t="str">
@@ -1746,6 +1860,10 @@
       <c r="I28" s="53"/>
       <c r="J28" s="53"/>
       <c r="K28" s="54"/>
+      <c r="L28" s="66" t="str">
+        <f><![CDATA[IF(AND(B28<>"",C28<>""),IF(IFERROR(MATCH(C28&" "&D28&" "&E28,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="61" t="str">
@@ -1761,6 +1879,10 @@
       <c r="I29" s="53"/>
       <c r="J29" s="53"/>
       <c r="K29" s="54"/>
+      <c r="L29" s="66" t="str">
+        <f><![CDATA[IF(AND(B29<>"",C29<>""),IF(IFERROR(MATCH(C29&" "&D29&" "&E29,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="61" t="str">
@@ -1776,6 +1898,10 @@
       <c r="I30" s="53"/>
       <c r="J30" s="53"/>
       <c r="K30" s="54"/>
+      <c r="L30" s="66" t="str">
+        <f><![CDATA[IF(AND(B30<>"",C30<>""),IF(IFERROR(MATCH(C30&" "&D30&" "&E30,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="61" t="str">
@@ -1791,6 +1917,10 @@
       <c r="I31" s="53"/>
       <c r="J31" s="53"/>
       <c r="K31" s="54"/>
+      <c r="L31" s="66" t="str">
+        <f><![CDATA[IF(AND(B31<>"",C31<>""),IF(IFERROR(MATCH(C31&" "&D31&" "&E31,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="61" t="str">
@@ -1806,8 +1936,12 @@
       <c r="I32" s="53"/>
       <c r="J32" s="53"/>
       <c r="K32" s="54"/>
-    </row>
-    <row r="33" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L32" s="66" t="str">
+        <f><![CDATA[IF(AND(B32<>"",C32<>""),IF(IFERROR(MATCH(C32&" "&D32&" "&E32,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1821,8 +1955,12 @@
       <c r="I33" s="53"/>
       <c r="J33" s="53"/>
       <c r="K33" s="54"/>
-    </row>
-    <row r="34" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L33" s="66" t="str">
+        <f><![CDATA[IF(AND(B33<>"",C33<>""),IF(IFERROR(MATCH(C33&" "&D33&" "&E33,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1836,8 +1974,12 @@
       <c r="I34" s="53"/>
       <c r="J34" s="53"/>
       <c r="K34" s="54"/>
-    </row>
-    <row r="35" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L34" s="66" t="str">
+        <f><![CDATA[IF(AND(B34<>"",C34<>""),IF(IFERROR(MATCH(C34&" "&D34&" "&E34,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1851,8 +1993,12 @@
       <c r="I35" s="53"/>
       <c r="J35" s="53"/>
       <c r="K35" s="54"/>
-    </row>
-    <row r="36" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L35" s="66" t="str">
+        <f><![CDATA[IF(AND(B35<>"",C35<>""),IF(IFERROR(MATCH(C35&" "&D35&" "&E35,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1866,8 +2012,12 @@
       <c r="I36" s="53"/>
       <c r="J36" s="53"/>
       <c r="K36" s="54"/>
-    </row>
-    <row r="37" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L36" s="66" t="str">
+        <f><![CDATA[IF(AND(B36<>"",C36<>""),IF(IFERROR(MATCH(C36&" "&D36&" "&E36,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1881,8 +2031,12 @@
       <c r="I37" s="53"/>
       <c r="J37" s="53"/>
       <c r="K37" s="54"/>
-    </row>
-    <row r="38" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L37" s="66" t="str">
+        <f><![CDATA[IF(AND(B37<>"",C37<>""),IF(IFERROR(MATCH(C37&" "&D37&" "&E37,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1896,8 +2050,12 @@
       <c r="I38" s="53"/>
       <c r="J38" s="53"/>
       <c r="K38" s="54"/>
-    </row>
-    <row r="39" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L38" s="66" t="str">
+        <f><![CDATA[IF(AND(B38<>"",C38<>""),IF(IFERROR(MATCH(C38&" "&D38&" "&E38,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1911,8 +2069,12 @@
       <c r="I39" s="53"/>
       <c r="J39" s="53"/>
       <c r="K39" s="54"/>
-    </row>
-    <row r="40" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L39" s="66" t="str">
+        <f><![CDATA[IF(AND(B39<>"",C39<>""),IF(IFERROR(MATCH(C39&" "&D39&" "&E39,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1926,8 +2088,12 @@
       <c r="I40" s="53"/>
       <c r="J40" s="53"/>
       <c r="K40" s="54"/>
-    </row>
-    <row r="41" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L40" s="66" t="str">
+        <f><![CDATA[IF(AND(B40<>"",C40<>""),IF(IFERROR(MATCH(C40&" "&D40&" "&E40,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1941,8 +2107,12 @@
       <c r="I41" s="53"/>
       <c r="J41" s="53"/>
       <c r="K41" s="54"/>
-    </row>
-    <row r="42" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L41" s="66" t="str">
+        <f><![CDATA[IF(AND(B41<>"",C41<>""),IF(IFERROR(MATCH(C41&" "&D41&" "&E41,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1956,8 +2126,12 @@
       <c r="I42" s="53"/>
       <c r="J42" s="53"/>
       <c r="K42" s="54"/>
-    </row>
-    <row r="43" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L42" s="66" t="str">
+        <f><![CDATA[IF(AND(B42<>"",C42<>""),IF(IFERROR(MATCH(C42&" "&D42&" "&E42,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1971,8 +2145,12 @@
       <c r="I43" s="53"/>
       <c r="J43" s="53"/>
       <c r="K43" s="54"/>
-    </row>
-    <row r="44" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L43" s="66" t="str">
+        <f><![CDATA[IF(AND(B43<>"",C43<>""),IF(IFERROR(MATCH(C43&" "&D43&" "&E43,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1986,8 +2164,12 @@
       <c r="I44" s="53"/>
       <c r="J44" s="53"/>
       <c r="K44" s="54"/>
-    </row>
-    <row r="45" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L44" s="66" t="str">
+        <f><![CDATA[IF(AND(B44<>"",C44<>""),IF(IFERROR(MATCH(C44&" "&D44&" "&E44,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2001,8 +2183,12 @@
       <c r="I45" s="53"/>
       <c r="J45" s="53"/>
       <c r="K45" s="54"/>
-    </row>
-    <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L45" s="66" t="str">
+        <f><![CDATA[IF(AND(B45<>"",C45<>""),IF(IFERROR(MATCH(C45&" "&D45&" "&E45,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2016,8 +2202,12 @@
       <c r="I46" s="53"/>
       <c r="J46" s="53"/>
       <c r="K46" s="54"/>
-    </row>
-    <row r="47" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L46" s="66" t="str">
+        <f><![CDATA[IF(AND(B46<>"",C46<>""),IF(IFERROR(MATCH(C46&" "&D46&" "&E46,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2031,8 +2221,12 @@
       <c r="I47" s="53"/>
       <c r="J47" s="53"/>
       <c r="K47" s="54"/>
-    </row>
-    <row r="48" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L47" s="66" t="str">
+        <f><![CDATA[IF(AND(B47<>"",C47<>""),IF(IFERROR(MATCH(C47&" "&D47&" "&E47,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2046,8 +2240,12 @@
       <c r="I48" s="53"/>
       <c r="J48" s="53"/>
       <c r="K48" s="54"/>
-    </row>
-    <row r="49" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L48" s="66" t="str">
+        <f><![CDATA[IF(AND(B48<>"",C48<>""),IF(IFERROR(MATCH(C48&" "&D48&" "&E48,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2061,8 +2259,12 @@
       <c r="I49" s="53"/>
       <c r="J49" s="53"/>
       <c r="K49" s="54"/>
-    </row>
-    <row r="50" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L49" s="66" t="str">
+        <f><![CDATA[IF(AND(B49<>"",C49<>""),IF(IFERROR(MATCH(C49&" "&D49&" "&E49,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2076,8 +2278,12 @@
       <c r="I50" s="53"/>
       <c r="J50" s="53"/>
       <c r="K50" s="54"/>
-    </row>
-    <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L50" s="66" t="str">
+        <f><![CDATA[IF(AND(B50<>"",C50<>""),IF(IFERROR(MATCH(C50&" "&D50&" "&E50,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2091,8 +2297,12 @@
       <c r="I51" s="53"/>
       <c r="J51" s="53"/>
       <c r="K51" s="54"/>
-    </row>
-    <row r="52" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L51" s="66" t="str">
+        <f><![CDATA[IF(AND(B51<>"",C51<>""),IF(IFERROR(MATCH(C51&" "&D51&" "&E51,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2106,8 +2316,12 @@
       <c r="I52" s="53"/>
       <c r="J52" s="53"/>
       <c r="K52" s="54"/>
-    </row>
-    <row r="53" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L52" s="66" t="str">
+        <f><![CDATA[IF(AND(B52<>"",C52<>""),IF(IFERROR(MATCH(C52&" "&D52&" "&E52,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2121,8 +2335,12 @@
       <c r="I53" s="53"/>
       <c r="J53" s="53"/>
       <c r="K53" s="54"/>
-    </row>
-    <row r="54" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L53" s="66" t="str">
+        <f><![CDATA[IF(AND(B53<>"",C53<>""),IF(IFERROR(MATCH(C53&" "&D53&" "&E53,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2136,6 +2354,10 @@
       <c r="I54" s="58"/>
       <c r="J54" s="58"/>
       <c r="K54" s="59"/>
+      <c r="L54" s="66" t="str">
+        <f><![CDATA[IF(AND(B54<>"",C54<>""),IF(IFERROR(MATCH(C54&" "&D54&" "&E54,Лист1!E:E,0),"✅")="✅","✅","Уже существует"),"")]]></f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2159,29 +2381,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AFBA1-F3EC-4CF2-9738-0B223AFFD495}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="4" width="21.5703125" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" style="8" width="9.140625"/>
+    <col min="2" max="4" customWidth="true" style="8" width="21.5703125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="9.42578125"/>
+    <col min="6" max="16384" style="8" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="63" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C3" s="63" t="s">
         <v>1</v>
@@ -2190,103 +2413,144 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="8" t="s">
+    <row r="4">
+      <c r="B4" t="s" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="C4" t="s" s="8">
         <v>23</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D4" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E4" t="s" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="5">
+      <c r="B5" t="s" s="8">
         <v>26</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C5" t="s" s="8">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D5" t="s" s="8">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="E5" t="s" s="8">
         <v>29</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="8" t="s">
+    </row>
+    <row r="6">
+      <c r="B6" t="s" s="8">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="C6" t="s" s="8">
         <v>31</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="D6" t="s" s="8">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="E6" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="8" t="s">
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="8">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="C7" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="E7" t="s" s="8">
         <v>36</v>
       </c>
-      <c r="D10" s="8" t="s">
+    </row>
+    <row r="8">
+      <c r="B8" t="s" s="8">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="C8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s" s="8">
         <v>38</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="E8" t="s" s="8">
         <v>39</v>
       </c>
-      <c r="D11" s="8" t="s">
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="C9" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s" s="8">
         <v>41</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="E9" t="s" s="8">
         <v>42</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>40</v>
+    </row>
+    <row r="10">
+      <c r="B10" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s" s="8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s" s="8">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="8">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s" s="8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s" s="8">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s" s="8">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2311,48 +2575,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="3.42578125"/>
+    <col min="2" max="2" customWidth="true" style="2" width="15.85546875"/>
+    <col min="3" max="3" customWidth="true" style="2" width="15.7109375"/>
+    <col min="4" max="4" customWidth="true" style="2" width="19.0"/>
+    <col min="5" max="5" customWidth="true" style="2" width="22.0"/>
+    <col min="6" max="6" customWidth="true" style="7" width="28.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="14.42578125"/>
+    <col min="8" max="8" customWidth="true" style="7" width="23.42578125"/>
+    <col min="9" max="16384" style="2" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
@@ -3275,45 +3539,45 @@
       <c r="F32" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="68" t="s">
+      <c r="A34" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67" t="s">
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="H34" s="67"/>
+      <c r="H34" s="70"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67" t="s">
+      <c r="A35" s="71"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="67"/>
+      <c r="H35" s="70"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67" t="str">
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70" t="str">
         <f ca="1">"Дата: " &amp; TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
         <v>Дата: 21.03.2023</v>
       </c>
-      <c r="H36" s="67"/>
+      <c r="H36" s="70"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>

</xml_diff>